<commit_message>
GoodInfo_v2 - 2021.12.02 未完成
</commit_message>
<xml_diff>
--- a/未實現分析.xlsx
+++ b/未實現分析.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,16 @@
         <v>5.03</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2021-12-02</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2021.12.06 未完成
</commit_message>
<xml_diff>
--- a/未實現分析.xlsx
+++ b/未實現分析.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +469,14 @@
         <v>0.73</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>44536</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>